<commit_message>
Update project name and add MIT license
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,11 +436,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>crema de leche 200g</t>
+          <t>azúcar</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5920.6</v>
+        <v>3753.876470588235</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>huevos</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2679.706666666666</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>leche semidesnatada</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>21982.638</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>aceite vegetal</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10260.66304347826</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>cacao en polvo 32%</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>No prices found</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>harina 1kg</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1474.8125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>polvo de hornear</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5656.67</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sal</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3033.001034482759</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>margarina</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>7329.649230769231</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>leche condensada</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4797.56875</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>crema de leche</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6428.746551724138</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cacao en polvo 50%</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>No prices found</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>granulado de chocolate</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9761.155999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>